<commit_message>
Lots of industry fixes for 2046/2050 runs
OTH:

added NCAP BND of 0 to address the issue of no new capacity on single tech demands/services causing backstop.

NMM
added same as above for bricks, glass, lime,

IS
fixed PRC_RESID issue and interpolation.
adjusted lower bound for scrap EAF production. for Eb calib.
same for coke ovens - this was causing backstop for manganese

ALM
PRCRESID - new shutdown profile added so gradually declines.
Added ncap bnd lower zero so that it can build new potlines.

FA:
PRCRESID - gradual decline in capacity.

IPP:
removed PRC_RESID of zero in BY as this causes NCAP_BND of zero to be generated.
error on new PULPD techs input sheet - was set to produce IPPULP which should be IPPULPD.
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-ALM.xlsx
+++ b/vt_REGION1_IND-ALM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32A25DF-DC2F-48B9-8B57-3D7CBD2E37FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC33BE5-5202-42AA-923A-049789E27335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="4635" windowWidth="20460" windowHeight="14700" tabRatio="796" firstSheet="4" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" firstSheet="4" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Production and Capacities" sheetId="62" r:id="rId1"/>
@@ -286,7 +286,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="390">
   <si>
     <t>Comment</t>
   </si>
@@ -1469,7 +1469,7 @@
     <t>NCAP_AF</t>
   </si>
   <si>
-    <t>ACT_BND~LO</t>
+    <t>NCAP_BND~LO~2017</t>
   </si>
 </sst>
 </file>
@@ -15079,13 +15079,13 @@
   <sheetPr codeName="Sheet30">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="N8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="7" topLeftCell="J8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="V8" sqref="V8"/>
+      <selection pane="bottomRight" activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15096,14 +15096,14 @@
     <col min="4" max="4" width="8.5703125" style="12" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="12" customWidth="1"/>
     <col min="6" max="6" width="8.28515625" style="12" customWidth="1"/>
-    <col min="7" max="16" width="9.140625" style="12"/>
-    <col min="17" max="17" width="7.85546875" style="12" customWidth="1"/>
-    <col min="18" max="18" width="7.5703125" style="12" customWidth="1"/>
+    <col min="7" max="18" width="9.140625" style="12"/>
     <col min="19" max="19" width="7.85546875" style="12" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="12"/>
+    <col min="20" max="20" width="7.5703125" style="12" customWidth="1"/>
+    <col min="21" max="21" width="7.85546875" style="12" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="200" t="str">
         <f ca="1">IF(INDEX(Index!$E$6:$E$37,MATCH(A2,Index!$D$6:$D$37,0))=1,LEFT(A2,SEARCH("_",A2)-1),"")</f>
         <v>ProcData</v>
@@ -15116,7 +15116,7 @@
       <c r="E1" s="38"/>
       <c r="F1" s="38"/>
     </row>
-    <row r="2" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="201" t="str">
         <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>ProcData_ALM</v>
@@ -15128,8 +15128,10 @@
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
       <c r="H2" s="38"/>
-    </row>
-    <row r="3" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+    </row>
+    <row r="3" spans="1:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="38"/>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -15139,36 +15141,38 @@
       <c r="G3" s="99" t="s">
         <v>138</v>
       </c>
-      <c r="H3" s="99" t="s">
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99" t="s">
         <v>138</v>
       </c>
-      <c r="I3" s="99" t="s">
+      <c r="K3" s="99" t="s">
         <v>143</v>
       </c>
-      <c r="J3" s="99" t="s">
+      <c r="L3" s="99" t="s">
         <v>165</v>
       </c>
-      <c r="K3" s="99"/>
-      <c r="L3" s="99" t="s">
-        <v>167</v>
-      </c>
-      <c r="M3" s="99" t="s">
-        <v>167</v>
-      </c>
+      <c r="M3" s="99"/>
       <c r="N3" s="99" t="s">
         <v>167</v>
       </c>
       <c r="O3" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="P3" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q3" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="R3" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="Q3" s="12" t="s">
+      <c r="S3" s="12" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="38"/>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
@@ -15182,43 +15186,49 @@
         <v>142</v>
       </c>
       <c r="I4" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="K4" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="L4" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="M4" s="45" t="s">
         <v>219</v>
-      </c>
-      <c r="L4" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="M4" s="45" t="s">
-        <v>168</v>
       </c>
       <c r="N4" s="45" t="s">
         <v>168</v>
       </c>
       <c r="O4" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="P4" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q4" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="P4" s="23" t="s">
+      <c r="R4" s="23" t="s">
         <v>124</v>
-      </c>
-      <c r="Q4" s="97" t="s">
-        <v>137</v>
-      </c>
-      <c r="R4" s="97" t="s">
-        <v>137</v>
       </c>
       <c r="S4" s="97" t="s">
         <v>137</v>
       </c>
-      <c r="T4" s="12" t="s">
+      <c r="T4" s="97" t="s">
+        <v>137</v>
+      </c>
+      <c r="U4" s="97" t="s">
+        <v>137</v>
+      </c>
+      <c r="V4" s="12" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="38"/>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
@@ -15229,39 +15239,45 @@
         <v>2017</v>
       </c>
       <c r="H5" s="45">
+        <v>2026</v>
+      </c>
+      <c r="I5" s="45">
+        <v>2027</v>
+      </c>
+      <c r="J5" s="45">
         <v>2028</v>
       </c>
-      <c r="L5" s="12" t="str">
+      <c r="N5" s="12" t="str">
         <f>EB_Exist!A9</f>
         <v>CO2SP</v>
       </c>
-      <c r="M5" s="12" t="str">
+      <c r="O5" s="12" t="str">
         <f>EB_Exist!A10</f>
         <v>CF4</v>
       </c>
-      <c r="N5" s="12" t="str">
+      <c r="P5" s="12" t="str">
         <f>EB_Exist!A11</f>
         <v>CF6</v>
       </c>
-      <c r="O5" s="40"/>
-      <c r="P5" s="23" t="str">
+      <c r="Q5" s="40"/>
+      <c r="R5" s="23" t="str">
         <f>E12</f>
         <v>IALM</v>
       </c>
-      <c r="Q5" s="12" t="str">
+      <c r="S5" s="12" t="str">
         <f>D9</f>
         <v>INDGAS</v>
       </c>
-      <c r="R5" s="12" t="str">
+      <c r="T5" s="12" t="str">
         <f>D10</f>
         <v>INDOLP</v>
       </c>
-      <c r="S5" s="12" t="str">
+      <c r="U5" s="12" t="str">
         <f>D11</f>
         <v>INFELC</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="38"/>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
@@ -15272,18 +15288,20 @@
       <c r="F6" s="38"/>
       <c r="G6" s="45"/>
       <c r="H6" s="45"/>
-      <c r="L6" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>118</v>
-      </c>
+      <c r="I6" s="45"/>
+      <c r="J6" s="45"/>
       <c r="N6" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="O6" s="40"/>
-    </row>
-    <row r="7" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O6" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q6" s="40"/>
+    </row>
+    <row r="7" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="38"/>
       <c r="B7" s="200" t="s">
         <v>368</v>
@@ -15301,69 +15319,77 @@
         <v>387</v>
       </c>
       <c r="G7" s="99" t="str">
-        <f t="shared" ref="G7:H7" si="0">IFERROR(REPLACE(G4,SEARCH("-",G4),1,"~"),G4)&amp;"~"&amp;G5</f>
+        <f t="shared" ref="G7:J7" si="0">IFERROR(REPLACE(G4,SEARCH("-",G4),1,"~"),G4)&amp;"~"&amp;G5</f>
         <v>PRC_RESID~2017</v>
       </c>
       <c r="H7" s="99" t="str">
+        <f t="shared" ref="H7" si="1">IFERROR(REPLACE(H4,SEARCH("-",H4),1,"~"),H4)&amp;"~"&amp;H5</f>
+        <v>PRC_RESID~2026</v>
+      </c>
+      <c r="I7" s="99" t="str">
+        <f t="shared" si="0"/>
+        <v>PRC_RESID~2027</v>
+      </c>
+      <c r="J7" s="99" t="str">
         <f t="shared" si="0"/>
         <v>PRC_RESID~2028</v>
       </c>
-      <c r="I7" s="99" t="str">
-        <f t="shared" ref="I7:K7" si="1">IFERROR(REPLACE(I4,SEARCH("-",I4),1,"~"),I4)</f>
+      <c r="K7" s="99" t="str">
+        <f t="shared" ref="K7:M7" si="2">IFERROR(REPLACE(K4,SEARCH("-",K4),1,"~"),K4)</f>
         <v>NCAP_FOM</v>
       </c>
-      <c r="J7" s="99" t="str">
-        <f t="shared" si="1"/>
+      <c r="L7" s="99" t="str">
+        <f t="shared" si="2"/>
         <v>NCAP_COST</v>
       </c>
-      <c r="K7" s="99" t="str">
-        <f t="shared" si="1"/>
+      <c r="M7" s="99" t="str">
+        <f t="shared" si="2"/>
         <v>NCAP_TLIFE</v>
       </c>
-      <c r="L7" s="99" t="str">
-        <f>"ENV_ACT~"&amp;L5</f>
+      <c r="N7" s="99" t="str">
+        <f>"ENV_ACT~"&amp;N5</f>
         <v>ENV_ACT~CO2SP</v>
       </c>
-      <c r="M7" s="99" t="str">
-        <f t="shared" ref="M7:N7" si="2">"ENV_ACT~"&amp;M5</f>
+      <c r="O7" s="99" t="str">
+        <f t="shared" ref="O7:P7" si="3">"ENV_ACT~"&amp;O5</f>
         <v>ENV_ACT~CF4</v>
       </c>
-      <c r="N7" s="99" t="str">
-        <f t="shared" si="2"/>
+      <c r="P7" s="99" t="str">
+        <f t="shared" si="3"/>
         <v>ENV_ACT~CF6</v>
       </c>
-      <c r="O7" s="99" t="str">
-        <f t="shared" ref="O7" si="3">IFERROR(REPLACE(O4,SEARCH("-",O4),1,"~"),O4)</f>
+      <c r="Q7" s="99" t="str">
+        <f t="shared" ref="Q7" si="4">IFERROR(REPLACE(Q4,SEARCH("-",Q4),1,"~"),Q4)</f>
         <v>PRC_CAPACT</v>
       </c>
-      <c r="P7" s="99" t="str">
-        <f>IFERROR(REPLACE(P4,SEARCH("-",P4),1,"~"),P4)</f>
+      <c r="R7" s="99" t="str">
+        <f>IFERROR(REPLACE(R4,SEARCH("-",R4),1,"~"),R4)</f>
         <v>PRC_ACTUNT</v>
       </c>
-      <c r="Q7" s="99" t="str">
-        <f>IFERROR(REPLACE(Q4,SEARCH("-",Q4),1,"~"),Q4)&amp;"~"&amp;2017</f>
+      <c r="S7" s="99" t="str">
+        <f>IFERROR(REPLACE(S4,SEARCH("-",S4),1,"~"),S4)&amp;"~"&amp;2017</f>
         <v>PRC_ACTFLO~2017</v>
       </c>
-      <c r="R7" s="99" t="str">
-        <f t="shared" ref="R7:S7" si="4">IFERROR(REPLACE(R4,SEARCH("-",R4),1,"~"),R4)&amp;"~"&amp;2017</f>
+      <c r="T7" s="99" t="str">
+        <f t="shared" ref="T7:U7" si="5">IFERROR(REPLACE(T4,SEARCH("-",T4),1,"~"),T4)&amp;"~"&amp;2017</f>
         <v>PRC_ACTFLO~2017</v>
       </c>
-      <c r="S7" s="99" t="str">
-        <f t="shared" si="4"/>
+      <c r="U7" s="99" t="str">
+        <f t="shared" si="5"/>
         <v>PRC_ACTFLO~2017</v>
       </c>
-      <c r="T7" s="99" t="str">
-        <f>IFERROR(REPLACE(T4,SEARCH("-",T4),1,"~"),T4)</f>
+      <c r="V7" s="99" t="str">
+        <f>IFERROR(REPLACE(V4,SEARCH("-",V4),1,"~"),V4)</f>
         <v>NCAP_START</v>
       </c>
-      <c r="U7" s="12" t="s">
+      <c r="W7" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="V7" s="12" t="s">
+      <c r="X7" s="12" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="str">
         <f>Processes_BASE!A8</f>
         <v>* Conversion technologies</v>
@@ -15373,8 +15399,10 @@
       <c r="F8" s="105"/>
       <c r="G8" s="100"/>
       <c r="H8" s="100"/>
-    </row>
-    <row r="9" spans="1:22" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I8" s="100"/>
+      <c r="J8" s="100"/>
+    </row>
+    <row r="9" spans="1:24" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="38" t="str">
         <f>Processes_BASE!B10</f>
@@ -15389,16 +15417,16 @@
         <v>INDGAS</v>
       </c>
       <c r="E9" s="106"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
       <c r="K9" s="96"/>
-      <c r="Q9" s="101">
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
+      <c r="S9" s="101">
         <f>EB_Exist!K6</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="R9" s="12"/>
-    </row>
-    <row r="10" spans="1:22" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T9" s="12"/>
+    </row>
+    <row r="10" spans="1:24" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="D10" s="106" t="str">
         <f>RES!E2</f>
@@ -15407,18 +15435,20 @@
       <c r="E10" s="106"/>
       <c r="G10" s="100"/>
       <c r="H10" s="100"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
+      <c r="I10" s="100"/>
+      <c r="J10" s="100"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
-      <c r="R10" s="129">
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="T10" s="129">
         <f>EB_Exist!K7</f>
         <v>3.26</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="D11" s="105" t="str">
         <f>RES!F2</f>
@@ -15426,18 +15456,20 @@
       </c>
       <c r="G11" s="100"/>
       <c r="H11" s="100"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
+      <c r="I11" s="100"/>
+      <c r="J11" s="100"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
-      <c r="S11" s="129">
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="U11" s="129">
         <f>EB_Exist!K8</f>
         <v>46.37</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -15451,46 +15483,51 @@
         <v>0.79999999999999993</v>
       </c>
       <c r="H12" s="100">
+        <v>0.8</v>
+      </c>
+      <c r="I12" s="100">
+        <v>0.4</v>
+      </c>
+      <c r="J12" s="100">
         <v>0</v>
       </c>
-      <c r="I12" s="127">
-        <f>2%*J12</f>
+      <c r="K12" s="127">
+        <f>2%*L12</f>
         <v>457.5</v>
       </c>
-      <c r="J12" s="12">
+      <c r="L12" s="12">
         <f>'Aluminium Data'!D7</f>
         <v>22875</v>
       </c>
-      <c r="K12" s="12">
+      <c r="M12" s="12">
         <v>6</v>
       </c>
-      <c r="L12" s="96">
+      <c r="N12" s="96">
         <f>EB_Exist!F9</f>
         <v>1640.7688481217385</v>
       </c>
-      <c r="M12" s="96">
+      <c r="O12" s="96">
         <f>EB_Exist!F10</f>
         <v>0.41016760505000449</v>
       </c>
-      <c r="N12" s="96">
+      <c r="P12" s="96">
         <f>EB_Exist!F11</f>
         <v>4.1062898593307487E-2</v>
       </c>
-      <c r="O12" s="12">
+      <c r="Q12" s="12">
         <v>1</v>
       </c>
-      <c r="P12" s="35">
+      <c r="R12" s="35">
         <v>1</v>
       </c>
-      <c r="U12" s="35">
+      <c r="W12" s="35">
         <v>1</v>
       </c>
-      <c r="V12" s="35">
-        <f>CommData_BASE!F15</f>
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X12" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="B13" s="38" t="str">
         <f>RES!M15</f>
@@ -15507,22 +15544,24 @@
       <c r="E13" s="105"/>
       <c r="G13" s="100"/>
       <c r="H13" s="100"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="100"/>
       <c r="K13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="Q13" s="126">
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="S13" s="126">
         <f>'Aluminium Data'!O32</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="R13" s="126"/>
-      <c r="S13" s="126"/>
-      <c r="T13" s="35">
+      <c r="T13" s="126"/>
+      <c r="U13" s="126"/>
+      <c r="V13" s="35">
         <v>2035</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -15536,16 +15575,18 @@
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
       <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="Q14" s="126"/>
-      <c r="R14" s="126">
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="S14" s="126"/>
+      <c r="T14" s="126">
         <f>'Aluminium Data'!O33</f>
         <v>3.26</v>
       </c>
-      <c r="S14" s="126"/>
-    </row>
-    <row r="15" spans="1:22" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U14" s="126"/>
+    </row>
+    <row r="15" spans="1:24" s="35" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -15562,51 +15603,53 @@
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
-      <c r="Q15" s="126"/>
-      <c r="R15" s="126"/>
-      <c r="S15" s="126">
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="S15" s="126"/>
+      <c r="T15" s="126"/>
+      <c r="U15" s="126">
         <f>'Aluminium Data'!O34</f>
         <v>56.57</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="106" t="str">
         <f>RES!O2</f>
         <v>IALM</v>
       </c>
-      <c r="I16" s="127">
-        <f>2%*J16</f>
+      <c r="K16" s="127">
+        <f>2%*L16</f>
         <v>587.5</v>
       </c>
-      <c r="J16" s="127">
+      <c r="L16" s="127">
         <f>'Aluminium Data'!L28</f>
         <v>29375</v>
       </c>
-      <c r="K16" s="127">
+      <c r="M16" s="127">
         <v>6</v>
-      </c>
-      <c r="L16" s="127">
-        <v>0</v>
-      </c>
-      <c r="M16" s="127">
-        <v>0</v>
       </c>
       <c r="N16" s="127">
         <v>0</v>
       </c>
-      <c r="O16" s="12">
+      <c r="O16" s="127">
+        <v>0</v>
+      </c>
+      <c r="P16" s="127">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="12">
         <v>1</v>
       </c>
-      <c r="P16" s="35">
+      <c r="R16" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="6:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F17" s="106"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
       <c r="R17" s="35"/>
       <c r="S17" s="35"/>
+      <c r="T17" s="35"/>
+      <c r="U17" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15945,7 +15988,7 @@
       </c>
       <c r="F9" s="106"/>
       <c r="H9" s="101">
-        <f>ProcData_ALM!Q9</f>
+        <f>ProcData_ALM!S9</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="I9" s="12"/>
@@ -15958,7 +16001,7 @@
       </c>
       <c r="F10" s="106"/>
       <c r="I10" s="101">
-        <f>ProcData_ALM!R10</f>
+        <f>ProcData_ALM!T10</f>
         <v>3.26</v>
       </c>
     </row>
@@ -15969,7 +16012,7 @@
         <v>INFELC</v>
       </c>
       <c r="J11" s="101">
-        <f>ProcData_ALM!S11</f>
+        <f>ProcData_ALM!U11</f>
         <v>46.37</v>
       </c>
       <c r="K11" s="35">

</xml_diff>

<commit_message>
Added Industry PAMS NEES scenario
Has full, and half NEES options.
Workbook could use a clean up. it was done very quickly.

A few tweaks to industry sheets.
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-ALM.xlsx
+++ b/vt_REGION1_IND-ALM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC33BE5-5202-42AA-923A-049789E27335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE22332D-1830-4AB1-BCAD-02A0C417BED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" firstSheet="4" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8775" yWindow="6975" windowWidth="21840" windowHeight="5400" tabRatio="796" firstSheet="4" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Production and Capacities" sheetId="62" r:id="rId1"/>
@@ -2820,7 +2820,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2952,7 +2952,7 @@
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3040,7 +3040,7 @@
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3084,7 +3084,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12449,8 +12449,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet">
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -12469,32 +12494,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets"/>
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12558,18 +12558,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -12578,7 +12578,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets"/>
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12608,18 +12608,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit">
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -12628,7 +12628,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit"/>
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12860,18 +12860,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="215041" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="215043" r:id="rId4" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>142875</xdr:rowOff>
               </to>
@@ -12880,7 +12880,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="215041" r:id="rId4" name="cmdSpecifySets"/>
+        <control shapeId="215043" r:id="rId4" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12910,18 +12910,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="215043" r:id="rId8" name="cmdCommUnit">
+        <control shapeId="215041" r:id="rId8" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>142875</xdr:rowOff>
               </to>
@@ -12930,7 +12930,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="215043" r:id="rId8" name="cmdCommUnit"/>
+        <control shapeId="215041" r:id="rId8" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13006,18 +13006,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -13026,7 +13026,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -13056,18 +13056,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -13076,7 +13076,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13155,18 +13155,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
+                <xdr:col>3</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -13175,7 +13175,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets"/>
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -13205,18 +13205,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
+                <xdr:col>4</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -13225,7 +13225,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit"/>
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13287,44 +13287,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet">
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -13332,7 +13307,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1"/>
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -13362,44 +13362,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter">
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -13407,7 +13382,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2"/>
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13589,52 +13589,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126981" r:id="rId4" name="cmdAddParamQualifier2">
+        <control shapeId="126977" r:id="rId4" name="cmdAddParameter">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126981" r:id="rId4" name="cmdAddParamQualifier2"/>
+        <control shapeId="126977" r:id="rId4" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126980" r:id="rId6" name="cmdCheckCommDataSheet">
+        <control shapeId="126978" r:id="rId6" name="cmdCommNameAndDesc">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126980" r:id="rId6" name="cmdCheckCommDataSheet"/>
+        <control shapeId="126978" r:id="rId6" name="cmdCommNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -13664,52 +13664,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126978" r:id="rId10" name="cmdCommNameAndDesc">
+        <control shapeId="126980" r:id="rId10" name="cmdCheckCommDataSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126978" r:id="rId10" name="cmdCommNameAndDesc"/>
+        <control shapeId="126980" r:id="rId10" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126977" r:id="rId12" name="cmdAddParameter">
+        <control shapeId="126981" r:id="rId12" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126977" r:id="rId12" name="cmdAddParameter"/>
+        <control shapeId="126981" r:id="rId12" name="cmdAddParamQualifier2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14154,18 +14154,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="128003" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="128001" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>142875</xdr:rowOff>
               </to>
@@ -14174,7 +14174,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="128003" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="128001" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -14204,18 +14204,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="128001" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="128003" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>142875</xdr:rowOff>
               </to>
@@ -14224,7 +14224,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="128001" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="128003" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14299,18 +14299,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -14319,57 +14344,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -14399,43 +14399,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -14444,32 +14419,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -15082,10 +15082,10 @@
   <dimension ref="A1:X17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="J8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="X8" sqref="X8"/>
+      <selection pane="bottomRight" activeCell="X12" sqref="W12:X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15660,18 +15660,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="157697" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="157703" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="157703" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="157702" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>847725</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -15680,57 +15705,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="157697" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="157702" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="157698" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="157701" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="157698" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="157699" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="157699" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="157701" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -15760,43 +15760,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="157701" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="157699" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
+                <xdr:col>5</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="157701" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="157702" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -15805,32 +15780,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="157702" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="157699" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="157703" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="157698" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="157703" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="157698" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="157697" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>847725</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="157697" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16077,18 +16077,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="199681" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="199687" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>1</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="199687" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="199686" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>847725</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -16097,57 +16122,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="199681" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="199686" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="199682" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="199685" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="199682" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="199683" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="199683" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="199685" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -16177,43 +16177,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="199685" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="199683" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
+                <xdr:col>5</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="199685" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="199686" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -16222,32 +16197,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="199686" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="199683" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="199687" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="199682" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="199687" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="199682" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="199681" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>847725</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="199681" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16537,8 +16537,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102407" r:id="rId8" name="cmdCommName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102407" r:id="rId8" name="cmdCommName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102402" r:id="rId16" name="cmdProcName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102402" r:id="rId16" name="cmdProcName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -16557,182 +16732,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102402" r:id="rId6" name="cmdProcName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102402" r:id="rId6" name="cmdProcName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102407" r:id="rId14" name="cmdCommName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102407" r:id="rId14" name="cmdCommName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2"/>
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16884,8 +16884,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet">
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -16904,82 +16979,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets"/>
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17056,8 +17056,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17076,232 +17301,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17368,8 +17368,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet">
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17388,182 +17563,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17641,8 +17641,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17661,232 +17886,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17976,8 +17976,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17996,232 +18221,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet"/>
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18301,8 +18301,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet">
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -18321,182 +18496,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18585,8 +18585,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears">
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -18605,232 +18830,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -20280,52 +20280,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId5">
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate"/>
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet"/>
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -20355,52 +20355,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId11">
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon"/>
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon"/>
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>